<commit_message>
feat: refactor client for FormClient
</commit_message>
<xml_diff>
--- a/聊天协议.xlsx
+++ b/聊天协议.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26327"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\liugangzuoye\code\netchathomework\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCC0CC41-D774-4D4F-A40D-14B494E71C67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView windowHeight="24320"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="82">
   <si>
     <t>头部</t>
   </si>
@@ -108,6 +102,9 @@
     <t>响应登录请求</t>
   </si>
   <si>
+    <t>结果代码 00:账号不存在, 01:密码不正确, 02:用户已登录, 03登录成功</t>
+  </si>
+  <si>
     <t>04|03</t>
   </si>
   <si>
@@ -198,7 +195,7 @@
     <t>响应添加好友</t>
   </si>
   <si>
-    <t>结果代码 00:账号不存在, 01:成功</t>
+    <t>结果代码 00:账号不存在, 01:成功, 02: 已经添加</t>
   </si>
   <si>
     <t>10|01</t>
@@ -284,39 +281,165 @@
   <si>
     <t>注：协议使用竖线|分隔，所以任何聊天消息、账号、昵称、密码都不允许存在|</t>
   </si>
-  <si>
-    <t>JUNLIN</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>SHENGQING</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>LIUGANG</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>DONE</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>结果代码 1:账号不存在, 2:密码不正确, 3:用户已登录, 0登录成功</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>1账号已经存在，0 注册成功</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+  </numFmts>
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -327,31 +450,202 @@
       <name val="Microsoft YaHei"/>
       <charset val="134"/>
     </font>
-    <font>
-      <sz val="9"/>
-      <name val="宋体"/>
-      <family val="3"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <family val="3"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="2">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -359,9 +653,251 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="24" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="18" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="14" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="18" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -372,24 +908,68 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="49">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="60% - 强调文字颜色 6" xfId="1" builtinId="52"/>
+    <cellStyle name="20% - 强调文字颜色 4" xfId="2" builtinId="42"/>
+    <cellStyle name="强调文字颜色 4" xfId="3" builtinId="41"/>
+    <cellStyle name="输入" xfId="4" builtinId="20"/>
+    <cellStyle name="40% - 强调文字颜色 3" xfId="5" builtinId="39"/>
+    <cellStyle name="20% - 强调文字颜色 3" xfId="6" builtinId="38"/>
+    <cellStyle name="货币" xfId="7" builtinId="4"/>
+    <cellStyle name="强调文字颜色 3" xfId="8" builtinId="37"/>
+    <cellStyle name="百分比" xfId="9" builtinId="5"/>
+    <cellStyle name="60% - 强调文字颜色 2" xfId="10" builtinId="36"/>
+    <cellStyle name="60% - 强调文字颜色 5" xfId="11" builtinId="48"/>
+    <cellStyle name="强调文字颜色 2" xfId="12" builtinId="33"/>
+    <cellStyle name="60% - 强调文字颜色 1" xfId="13" builtinId="32"/>
+    <cellStyle name="60% - 强调文字颜色 4" xfId="14" builtinId="44"/>
+    <cellStyle name="计算" xfId="15" builtinId="22"/>
+    <cellStyle name="强调文字颜色 1" xfId="16" builtinId="29"/>
+    <cellStyle name="适中" xfId="17" builtinId="28"/>
+    <cellStyle name="20% - 强调文字颜色 5" xfId="18" builtinId="46"/>
+    <cellStyle name="好" xfId="19" builtinId="26"/>
+    <cellStyle name="20% - 强调文字颜色 1" xfId="20" builtinId="30"/>
+    <cellStyle name="汇总" xfId="21" builtinId="25"/>
+    <cellStyle name="差" xfId="22" builtinId="27"/>
+    <cellStyle name="检查单元格" xfId="23" builtinId="23"/>
+    <cellStyle name="输出" xfId="24" builtinId="21"/>
+    <cellStyle name="标题 1" xfId="25" builtinId="16"/>
+    <cellStyle name="解释性文本" xfId="26" builtinId="53"/>
+    <cellStyle name="20% - 强调文字颜色 2" xfId="27" builtinId="34"/>
+    <cellStyle name="标题 4" xfId="28" builtinId="19"/>
+    <cellStyle name="货币[0]" xfId="29" builtinId="7"/>
+    <cellStyle name="40% - 强调文字颜色 4" xfId="30" builtinId="43"/>
+    <cellStyle name="千位分隔" xfId="31" builtinId="3"/>
+    <cellStyle name="已访问的超链接" xfId="32" builtinId="9"/>
+    <cellStyle name="标题" xfId="33" builtinId="15"/>
+    <cellStyle name="40% - 强调文字颜色 2" xfId="34" builtinId="35"/>
+    <cellStyle name="警告文本" xfId="35" builtinId="11"/>
+    <cellStyle name="60% - 强调文字颜色 3" xfId="36" builtinId="40"/>
+    <cellStyle name="注释" xfId="37" builtinId="10"/>
+    <cellStyle name="20% - 强调文字颜色 6" xfId="38" builtinId="50"/>
+    <cellStyle name="强调文字颜色 5" xfId="39" builtinId="45"/>
+    <cellStyle name="40% - 强调文字颜色 6" xfId="40" builtinId="51"/>
+    <cellStyle name="超链接" xfId="41" builtinId="8"/>
+    <cellStyle name="千位分隔[0]" xfId="42" builtinId="6"/>
+    <cellStyle name="标题 2" xfId="43" builtinId="17"/>
+    <cellStyle name="40% - 强调文字颜色 5" xfId="44" builtinId="47"/>
+    <cellStyle name="标题 3" xfId="45" builtinId="18"/>
+    <cellStyle name="强调文字颜色 6" xfId="46" builtinId="49"/>
+    <cellStyle name="40% - 强调文字颜色 1" xfId="47" builtinId="31"/>
+    <cellStyle name="链接单元格" xfId="48" builtinId="24"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -676,28 +1256,28 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I17"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" outlineLevelCol="7"/>
   <cols>
-    <col min="4" max="5" width="24.21875" customWidth="1"/>
-    <col min="6" max="6" width="16.77734375" customWidth="1"/>
-    <col min="7" max="7" width="65" customWidth="1"/>
-    <col min="8" max="8" width="30.33203125" customWidth="1"/>
-    <col min="9" max="9" width="57.21875" customWidth="1"/>
+    <col min="4" max="4" width="24.1826923076923" customWidth="1"/>
+    <col min="5" max="5" width="16.7307692307692" customWidth="1"/>
+    <col min="6" max="6" width="65" customWidth="1"/>
+    <col min="7" max="7" width="30.3653846153846" customWidth="1"/>
+    <col min="8" max="8" width="57.1826923076923" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -710,23 +1290,20 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
-        <v>84</v>
+      <c r="E1" t="s">
+        <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:8">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
@@ -739,20 +1316,17 @@
       <c r="D2" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="F2" t="s">
+      <c r="E2" t="s">
         <v>12</v>
       </c>
+      <c r="G2" t="s">
+        <v>13</v>
+      </c>
       <c r="H2" t="s">
-        <v>13</v>
-      </c>
-      <c r="I2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:8">
       <c r="A3" s="1" t="s">
         <v>15</v>
       </c>
@@ -765,23 +1339,17 @@
       <c r="D3" t="s">
         <v>16</v>
       </c>
-      <c r="E3" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="F3" t="s">
+      <c r="E3" t="s">
         <v>17</v>
       </c>
-      <c r="G3" s="3" t="s">
-        <v>86</v>
+      <c r="G3" t="s">
+        <v>18</v>
       </c>
       <c r="H3" t="s">
-        <v>18</v>
-      </c>
-      <c r="I3" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:8">
       <c r="A4" s="1" t="s">
         <v>20</v>
       </c>
@@ -794,20 +1362,17 @@
       <c r="D4" t="s">
         <v>21</v>
       </c>
-      <c r="E4" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="F4" t="s">
+      <c r="E4" t="s">
         <v>22</v>
       </c>
+      <c r="G4" t="s">
+        <v>23</v>
+      </c>
       <c r="H4" t="s">
-        <v>23</v>
-      </c>
-      <c r="I4" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:8">
       <c r="A5" s="1" t="s">
         <v>25</v>
       </c>
@@ -820,25 +1385,22 @@
       <c r="D5" t="s">
         <v>26</v>
       </c>
-      <c r="E5" s="3" t="s">
-        <v>84</v>
+      <c r="E5" t="s">
+        <v>27</v>
       </c>
       <c r="F5" t="s">
-        <v>27</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>85</v>
+        <v>28</v>
+      </c>
+      <c r="G5" t="s">
+        <v>29</v>
       </c>
       <c r="H5" t="s">
-        <v>28</v>
-      </c>
-      <c r="I5" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:8">
       <c r="A6" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B6" t="s">
         <v>9</v>
@@ -847,24 +1409,21 @@
         <v>10</v>
       </c>
       <c r="D6" t="s">
-        <v>31</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="F6" t="s">
         <v>32</v>
       </c>
+      <c r="E6" t="s">
+        <v>33</v>
+      </c>
+      <c r="G6" t="s">
+        <v>34</v>
+      </c>
       <c r="H6" t="s">
-        <v>33</v>
-      </c>
-      <c r="I6" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:8">
       <c r="A7" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B7" t="s">
         <v>10</v>
@@ -873,24 +1432,21 @@
         <v>9</v>
       </c>
       <c r="D7" t="s">
-        <v>36</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="F7" t="s">
         <v>37</v>
       </c>
+      <c r="E7" t="s">
+        <v>38</v>
+      </c>
+      <c r="G7" t="s">
+        <v>39</v>
+      </c>
       <c r="H7" t="s">
-        <v>38</v>
-      </c>
-      <c r="I7" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:8">
       <c r="A8" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B8" t="s">
         <v>9</v>
@@ -899,24 +1455,21 @@
         <v>10</v>
       </c>
       <c r="D8" t="s">
-        <v>41</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="F8" t="s">
         <v>42</v>
       </c>
+      <c r="E8" t="s">
+        <v>43</v>
+      </c>
+      <c r="G8" t="s">
+        <v>44</v>
+      </c>
       <c r="H8" t="s">
-        <v>43</v>
-      </c>
-      <c r="I8" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:8">
       <c r="A9" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B9" t="s">
         <v>10</v>
@@ -925,24 +1478,21 @@
         <v>9</v>
       </c>
       <c r="D9" t="s">
-        <v>46</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="F9" t="s">
         <v>47</v>
       </c>
+      <c r="E9" t="s">
+        <v>48</v>
+      </c>
+      <c r="G9" t="s">
+        <v>49</v>
+      </c>
       <c r="H9" t="s">
-        <v>48</v>
-      </c>
-      <c r="I9" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:8">
       <c r="A10" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B10" t="s">
         <v>9</v>
@@ -951,24 +1501,21 @@
         <v>10</v>
       </c>
       <c r="D10" t="s">
-        <v>51</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="F10" t="s">
         <v>52</v>
       </c>
+      <c r="E10" t="s">
+        <v>53</v>
+      </c>
+      <c r="G10" t="s">
+        <v>54</v>
+      </c>
       <c r="H10" t="s">
-        <v>53</v>
-      </c>
-      <c r="I10" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:8">
       <c r="A11" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B11" t="s">
         <v>10</v>
@@ -977,27 +1524,24 @@
         <v>9</v>
       </c>
       <c r="D11" t="s">
-        <v>56</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>81</v>
+        <v>57</v>
+      </c>
+      <c r="E11" t="s">
+        <v>58</v>
       </c>
       <c r="F11" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="G11" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="H11" t="s">
-        <v>59</v>
-      </c>
-      <c r="I11" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:8">
       <c r="A12" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B12" t="s">
         <v>9</v>
@@ -1006,21 +1550,21 @@
         <v>10</v>
       </c>
       <c r="D12" t="s">
-        <v>62</v>
-      </c>
-      <c r="F12" t="s">
         <v>63</v>
       </c>
+      <c r="E12" t="s">
+        <v>64</v>
+      </c>
+      <c r="G12" t="s">
+        <v>65</v>
+      </c>
       <c r="H12" t="s">
-        <v>64</v>
-      </c>
-      <c r="I12" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
-    <row r="13" spans="1:9">
+    <row r="13" spans="1:8">
       <c r="A13" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B13" t="s">
         <v>10</v>
@@ -1029,21 +1573,21 @@
         <v>9</v>
       </c>
       <c r="D13" t="s">
-        <v>67</v>
-      </c>
-      <c r="F13" t="s">
         <v>68</v>
       </c>
+      <c r="E13" t="s">
+        <v>69</v>
+      </c>
+      <c r="G13" t="s">
+        <v>70</v>
+      </c>
       <c r="H13" t="s">
-        <v>69</v>
-      </c>
-      <c r="I13" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
-    <row r="14" spans="1:9">
+    <row r="14" spans="1:8">
       <c r="A14" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B14" t="s">
         <v>9</v>
@@ -1052,24 +1596,21 @@
         <v>10</v>
       </c>
       <c r="D14" t="s">
-        <v>72</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="F14" t="s">
         <v>73</v>
       </c>
+      <c r="E14" t="s">
+        <v>74</v>
+      </c>
+      <c r="G14" t="s">
+        <v>73</v>
+      </c>
       <c r="H14" t="s">
-        <v>72</v>
-      </c>
-      <c r="I14" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="15.6">
+    <row r="15" ht="17" spans="1:8">
       <c r="A15" s="1" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B15" t="s">
         <v>10</v>
@@ -1077,66 +1618,68 @@
       <c r="C15" t="s">
         <v>9</v>
       </c>
-      <c r="D15" t="s">
-        <v>76</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="F15" t="s">
+      <c r="D15" s="2" t="s">
         <v>77</v>
       </c>
+      <c r="E15" t="s">
+        <v>78</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>79</v>
+      </c>
       <c r="H15" t="s">
-        <v>78</v>
-      </c>
-      <c r="I15" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
-      <c r="A17" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
+    <row r="17" spans="1:5">
+      <c r="A17" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A17:F17"/>
+    <mergeCell ref="A17:E17"/>
   </mergeCells>
-  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8"/>
   <sheetData/>
-  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8"/>
   <sheetData/>
-  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>